<commit_message>
changes to example model
</commit_message>
<xml_diff>
--- a/Matlab/Model/Model_Example/SBTAB_example.xlsx
+++ b/Matlab/Model/Model_Example/SBTAB_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\GitHub\Thesis_Code\Subcellular_workflow\Matlab\Model\Model_Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8E1F2E-1C86-499F-9224-61C26B66F23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569D7F26-8687-4656-A642-275B1C1831F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="0" windowWidth="23440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15370" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="17" r:id="rId1"/>
@@ -5399,7 +5399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8F9FC7-54DA-446C-A9CE-D67030941336}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -12295,7 +12295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47ED9D72-CE40-4006-85E9-411567212DBE}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -15795,7 +15795,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16734,7 +16734,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
better handle of tolerance values
</commit_message>
<xml_diff>
--- a/Matlab/Model/Model_Example/SBTAB_example.xlsx
+++ b/Matlab/Model/Model_Example/SBTAB_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\GitHub\Thesis_Code\Subcellular_workflow\Matlab\Model\Model_Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6372CE-983C-4145-A0A7-653858CD70EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A2EE30-714C-4961-A213-39254E90E941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="51820" windowHeight="21100" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29910" yWindow="2220" windowWidth="17775" windowHeight="16950" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="17" r:id="rId1"/>
@@ -5403,14 +5403,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>487</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>489</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>490</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>491</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>493</v>
       </c>
@@ -5497,12 +5497,12 @@
       <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>367</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>368</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>369</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>370</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>371</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>372</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>373</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>374</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>375</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>376</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>377</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>0.31542692581064402</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>379</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>0.46070725175664701</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>380</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>0.40422650062265603</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>381</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>0.30820040556796402</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>382</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>0.25192870165967501</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>383</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>0.223528480675656</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>384</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>0.20934895243436599</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>385</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>0.202372016910351</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>386</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>0.19903759452126499</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>387</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>0.197509944897859</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>388</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>0.196859666866602</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>389</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>0.19662395198773</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>390</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>0.19657557454173</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>391</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>0.19660488201868401</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>392</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>0.196660410260488</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>393</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>0.196719200044288</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>394</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>0.196772017626933</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>395</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>0.19681603436103301</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>396</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>0.19685123753565001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>397</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>0.19687870469996899</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>0.19689980375187999</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>399</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>0.19691584749528801</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>400</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>0.19692796622352801</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>401</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>0.196937080502016</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>402</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>0.19694391627428101</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>403</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>0.19694903462405999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>404</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>0.19695286361635</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>405</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>0.19695572704895001</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>0.196957868469605</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>0.19695947039401099</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>408</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>0.1969606692874</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>409</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>0.196961567050012</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>410</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>0.19696223972584201</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>411</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>0.19696274405766201</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>412</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>0.19696312239699301</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>413</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>0.196963406370328</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>414</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>0.196963619611387</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>415</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>0.19696377979523</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>416</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>0.196963900152025</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>417</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>0.19696399059365899</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>418</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>0.19696405855258001</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>419</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>0.196964109606795</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>420</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>0.196964147945935</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>421</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>0.19696417671914301</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>422</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>0.19696419829502401</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>423</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.19696421445610199</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>424</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>0.19696422654443599</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>425</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>0.19696423557078799</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>426</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>0.19696424229655701</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>427</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>0.19696424729532</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>428</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>0.24592207256315399</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>429</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>0.33009381077716299</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>430</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>0.32122813853075199</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>431</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>0.26919703737072498</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>432</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>0.21995055112369999</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>433</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>0.17986125897880201</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>434</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>0.146856749933756</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>435</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>0.119657960330423</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>436</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>9.7335876167031196E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>437</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>7.9096253409625797E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>438</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>6.4244113761818503E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>439</v>
       </c>
@@ -7878,7 +7878,7 @@
         <v>5.2179632724644397E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>440</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>4.2394486359109002E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>441</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>3.4464440871395302E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>442</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>2.80394768571437E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>443</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>2.2833164885188099E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>444</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>1.8612446960075298E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>445</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>1.51884232207148E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>446</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>1.24083696925061E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>447</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>1.0148998385180401E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>448</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>449</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>450</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>451</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>452</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>453</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>454</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>455</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>456</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>457</v>
       </c>
@@ -8454,7 +8454,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>458</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>459</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>460</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>461</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>462</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>463</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>464</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>465</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>466</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>467</v>
       </c>
@@ -8788,9 +8788,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>469</v>
       </c>
@@ -8831,7 +8831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>470</v>
       </c>
@@ -8842,93 +8842,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8942,12 +8942,12 @@
       <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>269</v>
       </c>
@@ -9115,7 +9115,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>271</v>
       </c>
@@ -9179,7 +9179,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>272</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>273</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>275</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>276</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>277</v>
       </c>
@@ -9371,7 +9371,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>279</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>280</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>281</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>282</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>283</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>284</v>
       </c>
@@ -9595,7 +9595,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>285</v>
       </c>
@@ -9627,7 +9627,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>286</v>
       </c>
@@ -9659,7 +9659,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>287</v>
       </c>
@@ -9691,7 +9691,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>288</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>290</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>291</v>
       </c>
@@ -9819,7 +9819,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>292</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>293</v>
       </c>
@@ -9883,7 +9883,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>294</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>295</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>296</v>
       </c>
@@ -9979,7 +9979,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>297</v>
       </c>
@@ -10011,7 +10011,7 @@
         <v>0.424949531040685</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>298</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>0.57992353489743997</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>299</v>
       </c>
@@ -10075,7 +10075,7 @@
         <v>0.45814206735493201</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>300</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>0.31683036540409099</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>301</v>
       </c>
@@ -10139,7 +10139,7 @@
         <v>0.239267711497193</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>302</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>0.201669086957393</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>303</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>0.183565756689512</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>304</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>0.175081858861481</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>305</v>
       </c>
@@ -10267,7 +10267,7 @@
         <v>0.17117661260124001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>306</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>0.16941311880603599</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>307</v>
       </c>
@@ -10331,7 +10331,7 @@
         <v>0.1686412759823</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>308</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>0.168323910015718</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>309</v>
       </c>
@@ -10395,7 +10395,7 @@
         <v>0.168210994730877</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>310</v>
       </c>
@@ -10427,7 +10427,7 @@
         <v>0.16818660937743199</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>311</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>0.16819756379038101</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>312</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>0.16822002489794399</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>313</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>0.168243831739496</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>314</v>
       </c>
@@ -10555,7 +10555,7 @@
         <v>0.16826509820334601</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>315</v>
       </c>
@@ -10587,7 +10587,7 @@
         <v>0.16828272809699599</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>316</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>0.16829678733640499</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>317</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>0.32592962569218897</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>318</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>0.46497183876932002</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>319</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>0.420416344993159</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>320</v>
       </c>
@@ -10747,7 +10747,7 @@
         <v>0.31774739471284102</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>321</v>
       </c>
@@ -10779,7 +10779,7 @@
         <v>0.23641602550479601</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>322</v>
       </c>
@@ -10811,7 +10811,7 @@
         <v>0.17742155304497201</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>323</v>
       </c>
@@ -10843,7 +10843,7 @@
         <v>0.133966561854479</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>324</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>0.101591900882573</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>325</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>7.7332538329984504E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>326</v>
       </c>
@@ -10939,7 +10939,7 @@
         <v>5.90747943646091E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>327</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>4.5280512562575002E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>328</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>3.4820297919375597E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>329</v>
       </c>
@@ -11035,7 +11035,7 @@
         <v>2.6860342371436401E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>330</v>
       </c>
@@ -11067,7 +11067,7 @@
         <v>2.0782397796629201E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>331</v>
       </c>
@@ -11099,7 +11099,7 @@
         <v>1.6126243033288801E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>332</v>
       </c>
@@ -11131,7 +11131,7 @@
         <v>1.2547992294846501E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>333</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>334</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>335</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>336</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>337</v>
       </c>
@@ -11291,7 +11291,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>338</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>339</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>340</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>341</v>
       </c>
@@ -11419,7 +11419,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>342</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>343</v>
       </c>
@@ -11483,7 +11483,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>344</v>
       </c>
@@ -11515,7 +11515,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>345</v>
       </c>
@@ -11547,7 +11547,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>347</v>
       </c>
@@ -11611,7 +11611,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>348</v>
       </c>
@@ -11643,7 +11643,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>349</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>350</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>351</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>352</v>
       </c>
@@ -11771,7 +11771,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>353</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>354</v>
       </c>
@@ -11835,7 +11835,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>355</v>
       </c>
@@ -11867,7 +11867,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>356</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>357</v>
       </c>
@@ -11931,7 +11931,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -11963,7 +11963,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>359</v>
       </c>
@@ -11995,7 +11995,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>360</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>361</v>
       </c>
@@ -12059,7 +12059,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>362</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>363</v>
       </c>
@@ -12123,7 +12123,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>364</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>365</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>366</v>
       </c>
@@ -12232,9 +12232,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12242,7 +12242,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>469</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>470</v>
       </c>
@@ -12299,12 +12299,12 @@
       <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12312,7 +12312,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -12376,7 +12376,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -12408,7 +12408,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -12440,7 +12440,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>269</v>
       </c>
@@ -12472,7 +12472,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -12504,7 +12504,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>271</v>
       </c>
@@ -12536,7 +12536,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>272</v>
       </c>
@@ -12568,7 +12568,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>273</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -12632,7 +12632,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>275</v>
       </c>
@@ -12664,7 +12664,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>276</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>277</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -12760,7 +12760,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>279</v>
       </c>
@@ -12792,7 +12792,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>280</v>
       </c>
@@ -12824,7 +12824,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>281</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>282</v>
       </c>
@@ -12888,7 +12888,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>283</v>
       </c>
@@ -12920,7 +12920,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>284</v>
       </c>
@@ -12952,7 +12952,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>285</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>286</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>287</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>288</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -13112,7 +13112,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>290</v>
       </c>
@@ -13144,7 +13144,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>291</v>
       </c>
@@ -13176,7 +13176,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>292</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>293</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>294</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>295</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>296</v>
       </c>
@@ -13336,7 +13336,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>297</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>0.52800510499820696</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>298</v>
       </c>
@@ -13400,7 +13400,7 @@
         <v>0.65883319320030598</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>299</v>
       </c>
@@ -13432,7 +13432,7 @@
         <v>0.47537715496969501</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>300</v>
       </c>
@@ -13464,7 +13464,7 @@
         <v>0.28767427755667102</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>301</v>
       </c>
@@ -13496,7 +13496,7 @@
         <v>0.19418513178806401</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>302</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>0.153946582853598</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>303</v>
       </c>
@@ -13560,7 +13560,7 @@
         <v>0.13590891106799</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>304</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>0.12799842772814801</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>305</v>
       </c>
@@ -13624,7 +13624,7 @@
         <v>0.124553365421102</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>306</v>
       </c>
@@ -13656,7 +13656,7 @@
         <v>0.123043814220707</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>307</v>
       </c>
@@ -13688,7 +13688,7 @@
         <v>0.465965063641684</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>308</v>
       </c>
@@ -13720,7 +13720,7 @@
         <v>0.61813574483492995</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>309</v>
       </c>
@@ -13752,7 +13752,7 @@
         <v>0.47186287850834002</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>310</v>
       </c>
@@ -13784,7 +13784,7 @@
         <v>0.30163968896723897</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>311</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>0.19393222745550201</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>312</v>
       </c>
@@ -13848,7 +13848,7 @@
         <v>0.13024696131938099</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>313</v>
       </c>
@@ -13880,7 +13880,7 @@
         <v>8.9741897384261193E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>314</v>
       </c>
@@ -13912,7 +13912,7 @@
         <v>6.2888142454068902E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>315</v>
       </c>
@@ -13944,7 +13944,7 @@
         <v>4.4654553784441199E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>316</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>3.2056725930846998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>317</v>
       </c>
@@ -14008,7 +14008,7 @@
         <v>2.3231074081535599E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>318</v>
       </c>
@@ -14040,7 +14040,7 @@
         <v>1.6975852355672501E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>319</v>
       </c>
@@ -14072,7 +14072,7 @@
         <v>1.24977526807338E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>320</v>
       </c>
@@ -14104,7 +14104,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>321</v>
       </c>
@@ -14136,7 +14136,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>322</v>
       </c>
@@ -14168,7 +14168,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>323</v>
       </c>
@@ -14200,7 +14200,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>324</v>
       </c>
@@ -14232,7 +14232,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>325</v>
       </c>
@@ -14264,7 +14264,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>326</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>327</v>
       </c>
@@ -14328,7 +14328,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>328</v>
       </c>
@@ -14360,7 +14360,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>329</v>
       </c>
@@ -14392,7 +14392,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>330</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>331</v>
       </c>
@@ -14456,7 +14456,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>332</v>
       </c>
@@ -14488,7 +14488,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>333</v>
       </c>
@@ -14520,7 +14520,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>334</v>
       </c>
@@ -14552,7 +14552,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>335</v>
       </c>
@@ -14584,7 +14584,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>336</v>
       </c>
@@ -14616,7 +14616,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>337</v>
       </c>
@@ -14648,7 +14648,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>338</v>
       </c>
@@ -14680,7 +14680,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>339</v>
       </c>
@@ -14712,7 +14712,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>340</v>
       </c>
@@ -14744,7 +14744,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>341</v>
       </c>
@@ -14776,7 +14776,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>342</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>343</v>
       </c>
@@ -14840,7 +14840,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>344</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>345</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>347</v>
       </c>
@@ -14968,7 +14968,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>348</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>349</v>
       </c>
@@ -15032,7 +15032,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>350</v>
       </c>
@@ -15064,7 +15064,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>351</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>352</v>
       </c>
@@ -15128,7 +15128,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>353</v>
       </c>
@@ -15160,7 +15160,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>354</v>
       </c>
@@ -15192,7 +15192,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>355</v>
       </c>
@@ -15224,7 +15224,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>356</v>
       </c>
@@ -15256,7 +15256,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>357</v>
       </c>
@@ -15288,7 +15288,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>359</v>
       </c>
@@ -15352,7 +15352,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>360</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>361</v>
       </c>
@@ -15416,7 +15416,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>362</v>
       </c>
@@ -15448,7 +15448,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>363</v>
       </c>
@@ -15480,7 +15480,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>364</v>
       </c>
@@ -15512,7 +15512,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>365</v>
       </c>
@@ -15544,7 +15544,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>366</v>
       </c>
@@ -15585,17 +15585,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8529D666-C96A-4DE4-9C04-475075734218}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15603,7 +15603,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -15614,7 +15614,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -15625,7 +15625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>469</v>
       </c>
@@ -15636,7 +15636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>470</v>
       </c>
@@ -15647,93 +15647,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15747,9 +15747,9 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15757,7 +15757,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -15771,7 +15771,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>472</v>
       </c>
@@ -15798,14 +15798,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="98.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15813,7 +15813,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -15833,7 +15833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -15854,7 +15854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -15896,7 +15896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -15917,7 +15917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -15938,7 +15938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -15959,7 +15959,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -15990,18 +15990,18 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="125.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16009,7 +16009,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -16041,7 +16041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -16073,7 +16073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -16084,7 +16084,7 @@
         <v>44</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
         <f>FALSE()</f>
@@ -16105,7 +16105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -16137,7 +16137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -16169,7 +16169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -16201,7 +16201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -16233,7 +16233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -16274,31 +16274,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="56.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16306,7 +16306,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -16359,7 +16359,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -16387,7 +16387,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -16415,7 +16415,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -16443,7 +16443,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -16471,7 +16471,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -16499,7 +16499,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -16527,7 +16527,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -16555,7 +16555,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -16612,7 +16612,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -16640,7 +16640,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -16668,7 +16668,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -16696,7 +16696,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -16737,20 +16737,20 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16758,7 +16758,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -16790,7 +16790,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -16824,7 +16824,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -16858,7 +16858,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -16892,7 +16892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -16936,16 +16936,17 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16953,7 +16954,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -16994,7 +16995,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -17030,7 +17031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -17066,7 +17067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -17102,7 +17103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>498</v>
       </c>
@@ -17152,12 +17153,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17165,7 +17166,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -17197,7 +17198,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -17229,7 +17230,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -17261,7 +17262,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -17293,7 +17294,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -17325,7 +17326,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -17357,7 +17358,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -17389,7 +17390,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -17421,7 +17422,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -17453,7 +17454,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -17485,7 +17486,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -17517,7 +17518,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -17549,7 +17550,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -17581,7 +17582,7 @@
         <v>0.171348181731038</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -17613,7 +17614,7 @@
         <v>0.27896636672566699</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -17645,7 +17646,7 @@
         <v>0.27192474401599998</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>171</v>
       </c>
@@ -17677,7 +17678,7 @@
         <v>0.235833115809403</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -17709,7 +17710,7 @@
         <v>0.21372818008149</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -17741,7 +17742,7 @@
         <v>0.203076313464819</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -17773,7 +17774,7 @@
         <v>0.198268522025215</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -17805,7 +17806,7 @@
         <v>0.196367240194572</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -17837,7 +17838,7 @@
         <v>0.19584766699559999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>177</v>
       </c>
@@ -17869,7 +17870,7 @@
         <v>0.19593530641236701</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -17901,7 +17902,7 @@
         <v>0.19625090728340699</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -17933,7 +17934,7 @@
         <v>0.196617915942116</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>180</v>
       </c>
@@ -17965,7 +17966,7 @@
         <v>0.19696087489337399</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -17997,7 +17998,7 @@
         <v>0.19725308724526799</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>182</v>
       </c>
@@ -18029,7 +18030,7 @@
         <v>0.19749019397138101</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>183</v>
       </c>
@@ -18061,7 +18062,7 @@
         <v>0.197677127109982</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -18093,7 +18094,7 @@
         <v>0.19782187402041601</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -18125,7 +18126,7 @@
         <v>0.19793266022772099</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -18157,7 +18158,7 @@
         <v>0.198016812590386</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -18189,7 +18190,7 @@
         <v>0.198080419939936</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -18221,7 +18222,7 @@
         <v>0.198128348712032</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -18253,7 +18254,7 @@
         <v>0.19816439672501299</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -18285,7 +18286,7 @@
         <v>0.19819148294982999</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -18317,7 +18318,7 @@
         <v>0.19821182857594299</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -18349,7 +18350,7 @@
         <v>0.19822711274587199</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>193</v>
       </c>
@@ -18381,7 +18382,7 @@
         <v>0.19823859943818001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>194</v>
       </c>
@@ -18413,7 +18414,7 @@
         <v>0.198247237595189</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>195</v>
       </c>
@@ -18445,7 +18446,7 @@
         <v>0.198253738564931</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -18477,7 +18478,7 @@
         <v>0.19825863521692799</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>197</v>
       </c>
@@ -18509,7 +18510,7 @@
         <v>0.19826232667820801</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>198</v>
       </c>
@@ -18541,7 +18542,7 @@
         <v>0.19826511199354499</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>199</v>
       </c>
@@ -18573,7 +18574,7 @@
         <v>0.19826721535821601</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>200</v>
       </c>
@@ -18605,7 +18606,7 @@
         <v>0.198268804990234</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -18637,7 +18638,7 @@
         <v>0.19827000722785901</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>202</v>
       </c>
@@ -18669,7 +18670,7 @@
         <v>0.19827091705521499</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>203</v>
       </c>
@@ -18701,7 +18702,7 @@
         <v>0.198271605961509</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>204</v>
       </c>
@@ -18733,7 +18734,7 @@
         <v>0.19827212781200099</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>205</v>
       </c>
@@ -18765,7 +18766,7 @@
         <v>0.19827252323703001</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>206</v>
       </c>
@@ -18797,7 +18798,7 @@
         <v>0.19827282291630899</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>207</v>
       </c>
@@ -18829,7 +18830,7 @@
         <v>0.19827305003926199</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>208</v>
       </c>
@@ -18861,7 +18862,7 @@
         <v>0.198273222150327</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>209</v>
       </c>
@@ -18893,7 +18894,7 @@
         <v>0.19827335253469799</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>210</v>
       </c>
@@ -18925,7 +18926,7 @@
         <v>0.19827345126027901</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>211</v>
       </c>
@@ -18957,7 +18958,7 @@
         <v>0.19827352596215</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>212</v>
       </c>
@@ -18989,7 +18990,7 @@
         <v>0.198273582433908</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>213</v>
       </c>
@@ -19021,7 +19022,7 @@
         <v>0.198273625073974</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>214</v>
       </c>
@@ -19053,7 +19054,7 @@
         <v>0.19827365722283499</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>215</v>
       </c>
@@ -19085,7 +19086,7 @@
         <v>0.19827368141815699</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>216</v>
       </c>
@@ -19117,7 +19118,7 @@
         <v>0.198273699587973</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>217</v>
       </c>
@@ -19149,7 +19150,7 @@
         <v>0.19827371319711701</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>218</v>
       </c>
@@ -19181,7 +19182,7 @@
         <v>0.19827372335832799</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>219</v>
       </c>
@@ -19213,7 +19214,7 @@
         <v>0.19827373091660599</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>220</v>
       </c>
@@ -19245,7 +19246,7 @@
         <v>0.19827373651331201</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>221</v>
       </c>
@@ -19277,7 +19278,7 @@
         <v>0.19827374063490699</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>222</v>
       </c>
@@ -19309,7 +19310,7 @@
         <v>0.19827374365003</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>223</v>
       </c>
@@ -19341,7 +19342,7 @@
         <v>0.19827374583771301</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>224</v>
       </c>
@@ -19373,7 +19374,7 @@
         <v>0.198273747408866</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>225</v>
       </c>
@@ -19405,7 +19406,7 @@
         <v>0.19827374852263499</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>226</v>
       </c>
@@ -19437,7 +19438,7 @@
         <v>0.19827374929886099</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>227</v>
       </c>
@@ -19469,7 +19470,7 @@
         <v>0.19827374982756199</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>228</v>
       </c>
@@ -19501,7 +19502,7 @@
         <v>0.20453950363485901</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>229</v>
       </c>
@@ -19533,7 +19534,7 @@
         <v>0.219786276776955</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -19565,7 +19566,7 @@
         <v>0.20635886118493799</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>231</v>
       </c>
@@ -19597,7 +19598,7 @@
         <v>0.176959327612287</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>232</v>
       </c>
@@ -19629,7 +19630,7 @@
         <v>0.150071684079088</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>233</v>
       </c>
@@ -19661,7 +19662,7 @@
         <v>0.12775946559586401</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>234</v>
       </c>
@@ -19693,7 +19694,7 @@
         <v>0.108974226194618</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>235</v>
       </c>
@@ -19725,7 +19726,7 @@
         <v>9.2897697115325598E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>236</v>
       </c>
@@ -19757,7 +19758,7 @@
         <v>7.9073897479705405E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>237</v>
       </c>
@@ -19789,7 +19790,7 @@
         <v>6.7191327442757603E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>238</v>
       </c>
@@ -19821,7 +19822,7 @@
         <v>5.7001210590072703E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>239</v>
       </c>
@@ -19853,7 +19854,7 @@
         <v>4.8287809889611497E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>240</v>
       </c>
@@ -19885,7 +19886,7 @@
         <v>4.0858325328707097E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>241</v>
       </c>
@@ -19917,7 +19918,7 @@
         <v>3.4539703965574403E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>242</v>
       </c>
@@ -19949,7 +19950,7 @@
         <v>2.9177513831011099E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>243</v>
       </c>
@@ -19981,7 +19982,7 @@
         <v>2.46351453138349E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>244</v>
       </c>
@@ -20013,7 +20014,7 @@
         <v>2.0792823657473501E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>245</v>
       </c>
@@ -20045,7 +20046,7 @@
         <v>1.75463676481049E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>246</v>
       </c>
@@ -20077,7 +20078,7 @@
         <v>1.48057721117308E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>247</v>
       </c>
@@ -20109,7 +20110,7 @@
         <v>1.24937157736915E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>248</v>
       </c>
@@ -20141,7 +20142,7 @@
         <v>1.05440796887667E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>249</v>
       </c>
@@ -20173,7 +20174,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>250</v>
       </c>
@@ -20205,7 +20206,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>251</v>
       </c>
@@ -20237,7 +20238,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>252</v>
       </c>
@@ -20269,7 +20270,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>253</v>
       </c>
@@ -20301,7 +20302,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>254</v>
       </c>
@@ -20333,7 +20334,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>255</v>
       </c>
@@ -20365,7 +20366,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>256</v>
       </c>
@@ -20397,7 +20398,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>257</v>
       </c>
@@ -20443,9 +20444,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20453,7 +20454,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -20464,7 +20465,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>259</v>
       </c>
@@ -20475,7 +20476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>260</v>
       </c>
@@ -20486,7 +20487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>261</v>
       </c>

</xml_diff>